<commit_message>
Draft of Solution for task2 and refactoring
</commit_message>
<xml_diff>
--- a/Input_data_task_2/2. Task.xlsx
+++ b/Input_data_task_2/2. Task.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pahorvat\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loranc\Documents\CV\Nokia_Budapest\Tasks\Input_data_task_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A187B8A7-34DC-4D97-940A-C5EE7F4F276E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA9A6ED-6150-49CC-8AD6-57AE7747EBED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3EAFAB75-5C67-4135-B17B-1A8C338DCBE3}"/>
+    <workbookView xWindow="18090" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{3EAFAB75-5C67-4135-B17B-1A8C338DCBE3}"/>
   </bookViews>
   <sheets>
     <sheet name="2.task" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="11">
   <si>
     <t>FG-AA123456</t>
   </si>
@@ -92,54 +92,6 @@
   </si>
   <si>
     <t>Confirmed Delivery ETA</t>
-  </si>
-  <si>
-    <t>202301</t>
-  </si>
-  <si>
-    <t>202302</t>
-  </si>
-  <si>
-    <t>202303</t>
-  </si>
-  <si>
-    <t>202304</t>
-  </si>
-  <si>
-    <t>202305</t>
-  </si>
-  <si>
-    <t>202306</t>
-  </si>
-  <si>
-    <t>202307</t>
-  </si>
-  <si>
-    <t>202308</t>
-  </si>
-  <si>
-    <t>202309</t>
-  </si>
-  <si>
-    <t>202310</t>
-  </si>
-  <si>
-    <t>202311</t>
-  </si>
-  <si>
-    <t>202312</t>
-  </si>
-  <si>
-    <t>202313</t>
-  </si>
-  <si>
-    <t>202314</t>
-  </si>
-  <si>
-    <t>202315</t>
-  </si>
-  <si>
-    <t>202316</t>
   </si>
 </sst>
 </file>
@@ -929,7 +881,7 @@
   <dimension ref="A1:BD26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="AL26" sqref="AL26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,13 +890,21 @@
     <col min="3" max="3" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" customWidth="1"/>
     <col min="18" max="26" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="27" max="31" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="32" max="39" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="43" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11" customWidth="1"/>
+    <col min="41" max="42" width="11.85546875" customWidth="1"/>
+    <col min="43" max="43" width="10.85546875" customWidth="1"/>
     <col min="44" max="48" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="49" max="52" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="53" max="55" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.28515625" customWidth="1"/>
+    <col min="54" max="54" width="10.140625" customWidth="1"/>
+    <col min="55" max="55" width="9.5703125" customWidth="1"/>
     <col min="56" max="56" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1021,211 +981,211 @@
       </c>
       <c r="E2" s="10">
         <f ca="1">TODAY()-WEEKDAY(TODAY(),2)+1</f>
-        <v>45495</v>
+        <v>45628</v>
       </c>
       <c r="F2" s="10">
         <f t="shared" ref="F2:BD2" ca="1" si="0">E2+7</f>
-        <v>45502</v>
+        <v>45635</v>
       </c>
       <c r="G2" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45509</v>
+        <f ca="1">F2+7</f>
+        <v>45642</v>
       </c>
       <c r="H2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45516</v>
+        <v>45649</v>
       </c>
       <c r="I2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45523</v>
+        <v>45656</v>
       </c>
       <c r="J2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45530</v>
+        <v>45663</v>
       </c>
       <c r="K2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45537</v>
+        <v>45670</v>
       </c>
       <c r="L2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45544</v>
+        <v>45677</v>
       </c>
       <c r="M2" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45551</v>
+        <f ca="1">L2+7</f>
+        <v>45684</v>
       </c>
       <c r="N2" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45558</v>
+        <f ca="1">M2+7</f>
+        <v>45691</v>
       </c>
       <c r="O2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45565</v>
+        <v>45698</v>
       </c>
       <c r="P2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45572</v>
+        <v>45705</v>
       </c>
       <c r="Q2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45579</v>
+        <v>45712</v>
       </c>
       <c r="R2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45586</v>
+        <v>45719</v>
       </c>
       <c r="S2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45593</v>
+        <v>45726</v>
       </c>
       <c r="T2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45600</v>
+        <v>45733</v>
       </c>
       <c r="U2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45607</v>
+        <v>45740</v>
       </c>
       <c r="V2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45614</v>
+        <v>45747</v>
       </c>
       <c r="W2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45621</v>
+        <v>45754</v>
       </c>
       <c r="X2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45628</v>
+        <v>45761</v>
       </c>
       <c r="Y2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45635</v>
+        <v>45768</v>
       </c>
       <c r="Z2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45642</v>
+        <v>45775</v>
       </c>
       <c r="AA2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45649</v>
+        <v>45782</v>
       </c>
       <c r="AB2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45656</v>
+        <v>45789</v>
       </c>
       <c r="AC2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45663</v>
+        <v>45796</v>
       </c>
       <c r="AD2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45670</v>
+        <v>45803</v>
       </c>
       <c r="AE2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45677</v>
+        <v>45810</v>
       </c>
       <c r="AF2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45684</v>
+        <v>45817</v>
       </c>
       <c r="AG2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45691</v>
+        <v>45824</v>
       </c>
       <c r="AH2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45698</v>
+        <v>45831</v>
       </c>
       <c r="AI2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45705</v>
+        <v>45838</v>
       </c>
       <c r="AJ2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45712</v>
+        <v>45845</v>
       </c>
       <c r="AK2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45719</v>
+        <v>45852</v>
       </c>
       <c r="AL2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45726</v>
+        <v>45859</v>
       </c>
       <c r="AM2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45733</v>
+        <v>45866</v>
       </c>
       <c r="AN2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45740</v>
+        <v>45873</v>
       </c>
       <c r="AO2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45747</v>
+        <v>45880</v>
       </c>
       <c r="AP2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45754</v>
+        <v>45887</v>
       </c>
       <c r="AQ2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45761</v>
+        <v>45894</v>
       </c>
       <c r="AR2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45768</v>
+        <v>45901</v>
       </c>
       <c r="AS2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45775</v>
+        <v>45908</v>
       </c>
       <c r="AT2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45782</v>
+        <v>45915</v>
       </c>
       <c r="AU2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45789</v>
+        <v>45922</v>
       </c>
       <c r="AV2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45796</v>
+        <v>45929</v>
       </c>
       <c r="AW2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45803</v>
+        <v>45936</v>
       </c>
       <c r="AX2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45810</v>
+        <v>45943</v>
       </c>
       <c r="AY2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45817</v>
+        <v>45950</v>
       </c>
       <c r="AZ2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45824</v>
+        <v>45957</v>
       </c>
       <c r="BA2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45831</v>
+        <v>45964</v>
       </c>
       <c r="BB2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45838</v>
+        <v>45971</v>
       </c>
       <c r="BC2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45845</v>
+        <v>45978</v>
       </c>
       <c r="BD2" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45852</v>
+        <v>45985</v>
       </c>
     </row>
     <row r="3" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1239,194 +1199,211 @@
       </c>
       <c r="E3" s="15" t="str">
         <f ca="1">YEAR(E2)&amp;IF(LEN(WEEKNUM(E2)-1)=1,0&amp;WEEKNUM(E2)-1,WEEKNUM(E2)-1)</f>
-        <v>202429</v>
+        <v>202448</v>
       </c>
       <c r="F3" s="15" t="str">
-        <f t="shared" ref="F3:AM3" ca="1" si="1">YEAR(F2)&amp;IF(LEN(WEEKNUM(F2)-1)=1,0&amp;WEEKNUM(F2)-1,WEEKNUM(F2)-1)</f>
-        <v>202430</v>
+        <f t="shared" ref="F3:BD3" ca="1" si="1">YEAR(F2)&amp;IF(LEN(WEEKNUM(F2)-1)=1,0&amp;WEEKNUM(F2)-1,WEEKNUM(F2)-1)</f>
+        <v>202449</v>
       </c>
       <c r="G3" s="15" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>202431</v>
+        <f ca="1">YEAR(G2)&amp;IF(LEN(WEEKNUM(G2)-1)=1,0&amp;WEEKNUM(G2)-1,WEEKNUM(G2)-1)</f>
+        <v>202450</v>
       </c>
       <c r="H3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202432</v>
+        <v>202451</v>
       </c>
       <c r="I3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202433</v>
+        <v>202452</v>
       </c>
       <c r="J3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202434</v>
+        <v>202501</v>
       </c>
       <c r="K3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202435</v>
+        <v>202502</v>
       </c>
       <c r="L3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202436</v>
+        <v>202503</v>
       </c>
       <c r="M3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202437</v>
+        <v>202504</v>
       </c>
       <c r="N3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202438</v>
+        <v>202505</v>
       </c>
       <c r="O3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202439</v>
+        <v>202506</v>
       </c>
       <c r="P3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202440</v>
+        <v>202507</v>
       </c>
       <c r="Q3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202441</v>
+        <v>202508</v>
       </c>
       <c r="R3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202442</v>
+        <v>202509</v>
       </c>
       <c r="S3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202443</v>
+        <v>202510</v>
       </c>
       <c r="T3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202444</v>
+        <v>202511</v>
       </c>
       <c r="U3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202445</v>
+        <v>202512</v>
       </c>
       <c r="V3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202446</v>
+        <v>202513</v>
       </c>
       <c r="W3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202447</v>
+        <v>202514</v>
       </c>
       <c r="X3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202448</v>
+        <v>202515</v>
       </c>
       <c r="Y3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202449</v>
+        <v>202516</v>
       </c>
       <c r="Z3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202450</v>
+        <v>202517</v>
       </c>
       <c r="AA3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202451</v>
+        <v>202518</v>
       </c>
       <c r="AB3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202452</v>
+        <v>202519</v>
       </c>
       <c r="AC3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202501</v>
+        <v>202520</v>
       </c>
       <c r="AD3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202502</v>
+        <v>202521</v>
       </c>
       <c r="AE3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202503</v>
+        <v>202522</v>
       </c>
       <c r="AF3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202504</v>
+        <v>202523</v>
       </c>
       <c r="AG3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202505</v>
+        <v>202524</v>
       </c>
       <c r="AH3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202506</v>
+        <v>202525</v>
       </c>
       <c r="AI3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202507</v>
+        <v>202526</v>
       </c>
       <c r="AJ3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202508</v>
+        <v>202527</v>
       </c>
       <c r="AK3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202509</v>
+        <v>202528</v>
       </c>
       <c r="AL3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202510</v>
+        <v>202529</v>
       </c>
       <c r="AM3" s="15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>202511</v>
-      </c>
-      <c r="AN3" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="AO3" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP3" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="AQ3" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="AR3" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="AS3" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="AT3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="AU3" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="AV3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="AW3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="AX3" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="AY3" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="AZ3" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="BA3" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="BB3" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="BC3" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="BD3" s="15">
-        <v>202317</v>
+        <v>202530</v>
+      </c>
+      <c r="AN3" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>202531</v>
+      </c>
+      <c r="AO3" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>202532</v>
+      </c>
+      <c r="AP3" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>202533</v>
+      </c>
+      <c r="AQ3" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>202534</v>
+      </c>
+      <c r="AR3" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>202535</v>
+      </c>
+      <c r="AS3" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>202536</v>
+      </c>
+      <c r="AT3" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>202537</v>
+      </c>
+      <c r="AU3" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>202538</v>
+      </c>
+      <c r="AV3" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>202539</v>
+      </c>
+      <c r="AW3" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>202540</v>
+      </c>
+      <c r="AX3" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>202541</v>
+      </c>
+      <c r="AY3" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>202542</v>
+      </c>
+      <c r="AZ3" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>202543</v>
+      </c>
+      <c r="BA3" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>202544</v>
+      </c>
+      <c r="BB3" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>202545</v>
+      </c>
+      <c r="BC3" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>202546</v>
+      </c>
+      <c r="BD3" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>202547</v>
       </c>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.25">
@@ -4897,7 +4874,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="30">
-        <f t="shared" si="2"/>
+        <f>SUM(G5:G24)</f>
         <v>100</v>
       </c>
       <c r="H25" s="30">
@@ -5113,11 +5090,11 @@
         <v>66573</v>
       </c>
       <c r="G26" s="34">
-        <f t="shared" ref="G26:BD26" si="41">F26+F25-G4</f>
+        <f>F26+F25-G4</f>
         <v>65573</v>
       </c>
       <c r="H26" s="34">
-        <f t="shared" si="41"/>
+        <f t="shared" ref="G26:BD26" si="41">G26+G25-H4</f>
         <v>64673</v>
       </c>
       <c r="I26" s="34">

</xml_diff>